<commit_message>
xen plan rates updated
</commit_message>
<xml_diff>
--- a/Inputs/MSH_Health_Expat/info.xlsx
+++ b/Inputs/MSH_Health_Expat/info.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">NE_Dubai/AbuDhabi/</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-11-01</t>
+    <t xml:space="preserve">2025-01-01</t>
   </si>
   <si>
     <t xml:space="preserve">USD</t>
@@ -177,10 +177,10 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.01"/>

</xml_diff>